<commit_message>
Refactor cModelTable handling and improve error messages
- Standardizes key-value field usage via cType.KEYVAL,
- Enhances error reporting with new messages in cMessages
- Improves documentation and validation in cModelTable, cReadModelTable, and related classes.
- Updates CSV and JSON model examples for consistent field order and structure.
- Refactors cResourceData and cWasteData handling for better validation and error logging.
</commit_message>
<xml_diff>
--- a/Examples/cgam/cgam_model.xlsx
+++ b/Examples/cgam/cgam_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctorr\Documents\Proyectos\TaesLab\Examples\cgam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C60B55C-546B-4555-87CF-2751A50BD771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526E358A-F5E8-460D-9941-D5EA7D3DC231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="780" windowWidth="25740" windowHeight="14700" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PhysicalDiagram" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <definedNames>
     <definedName name="cgam_flows" localSheetId="2">Flows!$A$1:$B$13</definedName>
-    <definedName name="cgam_processes" localSheetId="3">Processes!$A$1:$E$7</definedName>
+    <definedName name="cgam_processes" localSheetId="3">Processes!$A$1:$D$7</definedName>
     <definedName name="cgam_sample" localSheetId="4">Exergy!$A$1:$C$13</definedName>
     <definedName name="tgas_c0" localSheetId="8">ResourcesCost!$A$1:$C$1</definedName>
     <definedName name="tgas_fmt" localSheetId="5">Format!$A$1:$D$7</definedName>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="75">
   <si>
     <t>key</t>
   </si>
@@ -323,6 +323,9 @@
   </si>
   <si>
     <t>noAPH</t>
+  </si>
+  <si>
+    <t>recycle</t>
   </si>
 </sst>
 </file>
@@ -1015,18 +1018,17 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>14</v>
@@ -1043,7 +1045,7 @@
         <v>15</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1051,7 +1053,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>66</v>
@@ -1060,7 +1062,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1068,7 +1070,7 @@
         <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>54</v>
@@ -1077,7 +1079,7 @@
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1085,7 +1087,7 @@
         <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -1094,7 +1096,7 @@
         <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1102,7 +1104,7 @@
         <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>63</v>
@@ -1111,7 +1113,7 @@
         <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1119,7 +1121,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
@@ -1128,7 +1130,7 @@
         <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1136,7 +1138,7 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -1145,7 +1147,7 @@
         <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1157,7 +1159,7 @@
           <x14:formula1>
             <xm:f>Validate!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E7</xm:sqref>
+          <xm:sqref>B2:B7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1578,7 +1580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+    <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1692,10 +1694,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1703,20 +1705,26 @@
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>47</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1742,7 +1750,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>